<commit_message>
trabalhando em kpis de estoque
</commit_message>
<xml_diff>
--- a/app/Dash_Logistica/kpis_luiz/planilha/WQ4 - Estoque Mercadorias Cliente WMS - cliente 1.xlsx
+++ b/app/Dash_Logistica/kpis_luiz/planilha/WQ4 - Estoque Mercadorias Cliente WMS - cliente 1.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hausz\Desktop\Projetos\2022\06_Junho\Backend_Flask\app\Dash_Logistica\kpis_luiz\planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FACC7D-4CE0-4A35-B4E5-A3A43DFF61D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DEA8B5-5884-4FE4-9D97-34E29A899314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WQ4 - Estoque Mercadorias Clien" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'WQ4 - Estoque Mercadorias Clien'!$A$1:$R$453</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="926">
   <si>
     <t>Cód. Merc.</t>
   </si>
@@ -2798,9 +2801,6 @@
   </si>
   <si>
     <t>Monoporosa Hexa Dgr Lux 18X21 Sense</t>
-  </si>
-  <si>
-    <t>Totais</t>
   </si>
 </sst>
 </file>
@@ -3365,7 +3365,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3390,9 +3390,6 @@
     </xf>
     <xf numFmtId="3" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3752,10 +3749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R454"/>
+  <dimension ref="A1:R453"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="B448" sqref="B448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4265,7 +4262,7 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5">
         <v>0</v>
@@ -5292,7 +5289,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>76</v>
       </c>
@@ -27340,53 +27337,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="454" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A454" s="4"/>
-      <c r="B454" s="4"/>
-      <c r="C454" s="4"/>
-      <c r="D454" s="5"/>
-      <c r="E454" s="9" t="s">
-        <v>926</v>
-      </c>
-      <c r="F454" s="5"/>
-      <c r="G454" s="5">
-        <v>0</v>
-      </c>
-      <c r="H454" s="5">
-        <v>0</v>
-      </c>
-      <c r="I454" s="5">
-        <v>0</v>
-      </c>
-      <c r="J454" s="7">
-        <v>40418</v>
-      </c>
-      <c r="K454" s="5">
-        <v>0</v>
-      </c>
-      <c r="L454" s="7">
-        <v>40418</v>
-      </c>
-      <c r="M454" s="5">
-        <v>0</v>
-      </c>
-      <c r="N454" s="7">
-        <v>4541</v>
-      </c>
-      <c r="O454" s="7">
-        <v>4541</v>
-      </c>
-      <c r="P454" s="7">
-        <v>4146</v>
-      </c>
-      <c r="Q454" s="5">
-        <v>395</v>
-      </c>
-      <c r="R454" s="8">
-        <v>35877</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:R453" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>